<commit_message>
Added L1 Wt files
</commit_message>
<xml_diff>
--- a/Data/Bandit paper Key.xlsx
+++ b/Data/Bandit paper Key.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gowustl-my.sharepoint.com/personal/murrell_wustl_edu/Documents/Documents/Github/Murrell2025/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gowustl-my.sharepoint.com/personal/sebastiana_wustl_edu/Documents/Documents/GitHub/Murrell2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34656A20-6417-4378-82CB-7C38FFE50D46}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85C2E5E-8E87-42EE-B55E-7E56D2C4685E}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="960" windowWidth="23505" windowHeight="13800" xr2:uid="{D69361D2-749D-4D5A-8D7C-5685B1F0A3DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D69361D2-749D-4D5A-8D7C-5685B1F0A3DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$162</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -721,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -739,6 +742,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +758,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1077,11 +1077,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF4FCBB-AC4B-4BE1-B463-C994B1598E3A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G123" sqref="G123:G142"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1170,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -1178,33 +1179,33 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="2">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H3" s="2">
-        <v>18.350000000000001</v>
+        <v>24.61</v>
       </c>
       <c r="J3" s="2">
-        <v>19.149999999999999</v>
+        <v>24.56</v>
       </c>
       <c r="K3" s="2">
-        <v>18.350000000000001</v>
+        <v>24.21</v>
       </c>
       <c r="L3" s="2">
-        <v>19.809999999999999</v>
+        <v>24.52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -1219,27 +1220,27 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="2">
-        <v>18.5</v>
+        <v>18.46</v>
       </c>
       <c r="J4" s="2">
-        <v>19.690000000000001</v>
+        <v>19.739999999999998</v>
       </c>
       <c r="K4" s="2">
-        <v>18.600000000000001</v>
+        <v>19.87</v>
       </c>
       <c r="L4" s="2">
-        <v>20.07</v>
+        <v>19.48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -1254,27 +1255,27 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H5" s="2">
-        <v>18.46</v>
+        <v>20.25</v>
       </c>
       <c r="J5" s="2">
-        <v>19.739999999999998</v>
+        <v>21.56</v>
       </c>
       <c r="K5" s="2">
-        <v>19.87</v>
+        <v>20.149999999999999</v>
       </c>
       <c r="L5" s="2">
-        <v>19.48</v>
+        <v>20.63</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1283,33 +1284,33 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="2">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H6" s="2">
-        <v>19.91</v>
+        <v>27.54</v>
       </c>
       <c r="J6" s="2">
-        <v>21.59</v>
+        <v>28.15</v>
       </c>
       <c r="K6" s="2">
-        <v>20.03</v>
+        <v>27.22</v>
       </c>
       <c r="L6" s="2">
-        <v>20.39</v>
+        <v>27.35</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -1318,33 +1319,33 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H7" s="2">
-        <v>18.48</v>
+        <v>26.44</v>
       </c>
       <c r="J7" s="2">
-        <v>19.05</v>
+        <v>26.37</v>
       </c>
       <c r="K7" s="2">
-        <v>18.84</v>
+        <v>25.59</v>
       </c>
       <c r="L7" s="2">
-        <v>19.68</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -1359,27 +1360,27 @@
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H8" s="2">
-        <v>19.95</v>
+        <v>19.239999999999998</v>
       </c>
       <c r="J8" s="2">
-        <v>20.89</v>
+        <v>19.309999999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>20.100000000000001</v>
+        <v>18.53</v>
       </c>
       <c r="L8" s="2">
-        <v>20.420000000000002</v>
+        <v>20.23</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1394,27 +1395,27 @@
         <v>10</v>
       </c>
       <c r="F9" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H9" s="2">
-        <v>17.53</v>
+        <v>19.91</v>
       </c>
       <c r="J9" s="2">
-        <v>19.03</v>
+        <v>21.59</v>
       </c>
       <c r="K9" s="2">
-        <v>18.21</v>
+        <v>20.03</v>
       </c>
       <c r="L9" s="2">
-        <v>20.079999999999998</v>
+        <v>20.39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1423,33 +1424,33 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="2">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H10" s="2">
-        <v>20.25</v>
+        <v>23.28</v>
       </c>
       <c r="J10" s="2">
-        <v>21.56</v>
+        <v>24.43</v>
       </c>
       <c r="K10" s="2">
-        <v>20.149999999999999</v>
+        <v>22.71</v>
       </c>
       <c r="L10" s="2">
-        <v>20.63</v>
+        <v>23.59</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -1458,33 +1459,33 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="2">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H11" s="2">
-        <v>19.239999999999998</v>
+        <v>26.74</v>
       </c>
       <c r="J11" s="2">
-        <v>19.309999999999999</v>
+        <v>26.88</v>
       </c>
       <c r="K11" s="2">
-        <v>18.53</v>
+        <v>25.92</v>
       </c>
       <c r="L11" s="2">
-        <v>20.23</v>
+        <v>26.05</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -1499,27 +1500,27 @@
         <v>10</v>
       </c>
       <c r="F12" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H12" s="2">
-        <v>26.74</v>
+        <v>26.66</v>
       </c>
       <c r="J12" s="2">
-        <v>26.88</v>
+        <v>26.44</v>
       </c>
       <c r="K12" s="2">
-        <v>25.92</v>
+        <v>25.4</v>
       </c>
       <c r="L12" s="2">
-        <v>26.05</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
@@ -1528,28 +1529,28 @@
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="2">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H13" s="2">
-        <v>26.66</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="J13" s="2">
-        <v>26.44</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="K13" s="2">
-        <v>25.4</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="L13" s="2">
-        <v>26</v>
+        <v>19.809999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1589,7 +1590,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -1598,33 +1599,33 @@
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="2">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H15" s="2">
-        <v>24.61</v>
+        <v>18.5</v>
       </c>
       <c r="J15" s="2">
-        <v>24.56</v>
+        <v>19.690000000000001</v>
       </c>
       <c r="K15" s="2">
-        <v>24.21</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="L15" s="2">
-        <v>24.52</v>
+        <v>20.07</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
@@ -1639,27 +1640,27 @@
         <v>10</v>
       </c>
       <c r="F16" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H16" s="2">
-        <v>23.28</v>
+        <v>26.96</v>
       </c>
       <c r="J16" s="2">
-        <v>24.43</v>
+        <v>27.54</v>
       </c>
       <c r="K16" s="2">
-        <v>22.71</v>
+        <v>26.16</v>
       </c>
       <c r="L16" s="2">
-        <v>23.59</v>
+        <v>25.54</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
@@ -1668,28 +1669,28 @@
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="2">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H17" s="2">
-        <v>26.96</v>
+        <v>19.95</v>
       </c>
       <c r="J17" s="2">
-        <v>27.54</v>
+        <v>20.89</v>
       </c>
       <c r="K17" s="2">
-        <v>26.16</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L17" s="2">
-        <v>25.54</v>
+        <v>20.420000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1764,7 +1765,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -1773,33 +1774,33 @@
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="2">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H20" s="2">
-        <v>27.54</v>
+        <v>17.53</v>
       </c>
       <c r="J20" s="2">
-        <v>28.15</v>
+        <v>19.03</v>
       </c>
       <c r="K20" s="2">
-        <v>27.22</v>
+        <v>18.21</v>
       </c>
       <c r="L20" s="2">
-        <v>27.35</v>
+        <v>20.079999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
@@ -1808,31 +1809,31 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="2">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H21" s="2">
-        <v>26.44</v>
+        <v>18.48</v>
       </c>
       <c r="J21" s="2">
-        <v>26.37</v>
+        <v>19.05</v>
       </c>
       <c r="K21" s="2">
-        <v>25.59</v>
+        <v>18.84</v>
       </c>
       <c r="L21" s="2">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19.68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>21.05</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>19.62</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1975,7 +1976,7 @@
         <v>19.38</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>17.850000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>18.350000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>17.86</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>19.64</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>19.98</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>25.66</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>23.02</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>27.32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>22.38</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>24.28</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>25.25</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>101</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>102</v>
       </c>
@@ -2603,7 +2604,7 @@
         <v>18.559999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>21.47</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>21.21</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>20.71</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>107</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>18.97</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>19.079999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>19.77</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -2907,7 +2908,7 @@
         <v>18.88</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>26.39</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>27.91</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>22.95</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>26.07</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>24.56</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>25.88</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>24.38</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -3325,9 +3326,9 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>38</v>
@@ -3336,36 +3337,36 @@
         <v>39</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F62" s="2">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H62" s="2">
-        <v>24.96</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="I62" s="2">
-        <v>24.34</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="J62" s="2">
-        <v>25.53</v>
+        <v>20.36</v>
       </c>
       <c r="K62" s="2">
-        <v>24.6</v>
+        <v>18.55</v>
       </c>
       <c r="L62" s="2">
-        <v>25.53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>57</v>
+        <v>19.41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>38</v>
@@ -3380,7 +3381,7 @@
         <v>10</v>
       </c>
       <c r="F63" s="2">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>85</v>
@@ -3389,21 +3390,21 @@
         <v>23.06</v>
       </c>
       <c r="I63" s="2">
-        <v>22.83</v>
+        <v>22.23</v>
       </c>
       <c r="J63" s="2">
-        <v>23.79</v>
+        <v>23.01</v>
       </c>
       <c r="K63" s="2">
-        <v>23.32</v>
+        <v>22.04</v>
       </c>
       <c r="L63" s="2">
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>56</v>
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>38</v>
@@ -3418,30 +3419,30 @@
         <v>10</v>
       </c>
       <c r="F64" s="2">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H64" s="2">
-        <v>28.22</v>
+        <v>24.77</v>
       </c>
       <c r="I64" s="2">
-        <v>26.99</v>
+        <v>23.89</v>
       </c>
       <c r="J64" s="2">
-        <v>28.16</v>
+        <v>24.12</v>
       </c>
       <c r="K64" s="2">
-        <v>27.15</v>
+        <v>23.51</v>
       </c>
       <c r="L64" s="2">
-        <v>26.41</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>55</v>
+        <v>23.76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>38</v>
@@ -3456,30 +3457,30 @@
         <v>10</v>
       </c>
       <c r="F65" s="2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H65" s="2">
-        <v>18.579999999999998</v>
+        <v>20.46</v>
       </c>
       <c r="I65" s="2">
-        <v>17.260000000000002</v>
+        <v>20.27</v>
       </c>
       <c r="J65" s="2">
-        <v>18.690000000000001</v>
+        <v>21.1</v>
       </c>
       <c r="K65" s="2">
-        <v>18.350000000000001</v>
+        <v>20.02</v>
       </c>
       <c r="L65" s="2">
-        <v>18.48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>54</v>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>38</v>
@@ -3494,30 +3495,30 @@
         <v>10</v>
       </c>
       <c r="F66" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H66" s="2">
-        <v>20.27</v>
+        <v>20.66</v>
       </c>
       <c r="I66" s="2">
-        <v>19.54</v>
+        <v>19.91</v>
       </c>
       <c r="J66" s="2">
-        <v>20.25</v>
+        <v>21.55</v>
       </c>
       <c r="K66" s="2">
-        <v>19.3</v>
+        <v>20.309999999999999</v>
       </c>
       <c r="L66" s="2">
-        <v>20.22</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>53</v>
+        <v>20.309999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>38</v>
@@ -3526,36 +3527,36 @@
         <v>39</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F67" s="2">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H67" s="2">
-        <v>25.91</v>
+        <v>20.28</v>
       </c>
       <c r="I67" s="2">
-        <v>24.79</v>
+        <v>19.22</v>
       </c>
       <c r="J67" s="2">
-        <v>26.04</v>
+        <v>20.05</v>
       </c>
       <c r="K67" s="2">
-        <v>25.42</v>
+        <v>19.7</v>
       </c>
       <c r="L67" s="2">
-        <v>24.83</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20.95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>38</v>
@@ -3570,30 +3571,30 @@
         <v>10</v>
       </c>
       <c r="F68" s="2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H68" s="2">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="I68" s="2">
+        <v>19.14</v>
+      </c>
+      <c r="J68" s="2">
+        <v>20.67</v>
+      </c>
+      <c r="K68" s="2">
         <v>19.079999999999998</v>
       </c>
-      <c r="I68" s="2">
-        <v>18.149999999999999</v>
-      </c>
-      <c r="J68" s="2">
-        <v>18.8</v>
-      </c>
-      <c r="K68" s="2">
-        <v>18.5</v>
-      </c>
       <c r="L68" s="2">
-        <v>18.86</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19.559999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>38</v>
@@ -3608,30 +3609,30 @@
         <v>10</v>
       </c>
       <c r="F69" s="2">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H69" s="2">
-        <v>27.11</v>
+        <v>24.74</v>
       </c>
       <c r="I69" s="2">
-        <v>25.47</v>
+        <v>23.87</v>
       </c>
       <c r="J69" s="2">
-        <v>26.88</v>
+        <v>25.07</v>
       </c>
       <c r="K69" s="2">
-        <v>26.22</v>
+        <v>23.61</v>
       </c>
       <c r="L69" s="2">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>38</v>
@@ -3646,30 +3647,30 @@
         <v>10</v>
       </c>
       <c r="F70" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H70" s="2">
-        <v>19.96</v>
+        <v>20.98</v>
       </c>
       <c r="I70" s="2">
-        <v>18.899999999999999</v>
+        <v>20.03</v>
       </c>
       <c r="J70" s="2">
-        <v>20.59</v>
+        <v>21.24</v>
       </c>
       <c r="K70" s="2">
-        <v>19.36</v>
+        <v>20.079999999999998</v>
       </c>
       <c r="L70" s="2">
-        <v>20.45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>21.11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>38</v>
@@ -3684,30 +3685,30 @@
         <v>10</v>
       </c>
       <c r="F71" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H71" s="2">
-        <v>27.08</v>
+        <v>26.92</v>
       </c>
       <c r="I71" s="2">
-        <v>20.420000000000002</v>
+        <v>26.24</v>
       </c>
       <c r="J71" s="2">
-        <v>27.11</v>
+        <v>27</v>
       </c>
       <c r="K71" s="2">
-        <v>27.21</v>
+        <v>25.56</v>
       </c>
       <c r="L71" s="2">
-        <v>26.94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26.04</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>38</v>
@@ -3722,30 +3723,30 @@
         <v>10</v>
       </c>
       <c r="F72" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H72" s="2">
-        <v>26.92</v>
+        <v>27.08</v>
       </c>
       <c r="I72" s="2">
-        <v>26.24</v>
+        <v>20.420000000000002</v>
       </c>
       <c r="J72" s="2">
-        <v>27</v>
+        <v>27.11</v>
       </c>
       <c r="K72" s="2">
-        <v>25.56</v>
+        <v>27.21</v>
       </c>
       <c r="L72" s="2">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26.94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>38</v>
@@ -3760,30 +3761,30 @@
         <v>10</v>
       </c>
       <c r="F73" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H73" s="2">
-        <v>20.98</v>
+        <v>19.96</v>
       </c>
       <c r="I73" s="2">
-        <v>20.03</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="J73" s="2">
-        <v>21.24</v>
+        <v>20.59</v>
       </c>
       <c r="K73" s="2">
-        <v>20.079999999999998</v>
+        <v>19.36</v>
       </c>
       <c r="L73" s="2">
-        <v>21.11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20.45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>38</v>
@@ -3798,30 +3799,30 @@
         <v>10</v>
       </c>
       <c r="F74" s="2">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H74" s="2">
-        <v>24.74</v>
+        <v>27.11</v>
       </c>
       <c r="I74" s="2">
-        <v>23.87</v>
+        <v>25.47</v>
       </c>
       <c r="J74" s="2">
-        <v>25.07</v>
+        <v>26.88</v>
       </c>
       <c r="K74" s="2">
-        <v>23.61</v>
+        <v>26.22</v>
       </c>
       <c r="L74" s="2">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>38</v>
@@ -3836,30 +3837,30 @@
         <v>10</v>
       </c>
       <c r="F75" s="2">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H75" s="2">
-        <v>19.350000000000001</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="I75" s="2">
-        <v>19.14</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="J75" s="2">
-        <v>20.67</v>
+        <v>18.8</v>
       </c>
       <c r="K75" s="2">
-        <v>19.079999999999998</v>
+        <v>18.5</v>
       </c>
       <c r="L75" s="2">
-        <v>19.559999999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18.86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>38</v>
@@ -3868,36 +3869,36 @@
         <v>39</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F76" s="2">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H76" s="2">
-        <v>20.28</v>
+        <v>25.91</v>
       </c>
       <c r="I76" s="2">
-        <v>19.22</v>
+        <v>24.79</v>
       </c>
       <c r="J76" s="2">
-        <v>20.05</v>
+        <v>26.04</v>
       </c>
       <c r="K76" s="2">
-        <v>19.7</v>
+        <v>25.42</v>
       </c>
       <c r="L76" s="2">
-        <v>20.95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>24.83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>38</v>
@@ -3912,30 +3913,30 @@
         <v>10</v>
       </c>
       <c r="F77" s="2">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H77" s="2">
-        <v>20.66</v>
+        <v>20.27</v>
       </c>
       <c r="I77" s="2">
-        <v>19.91</v>
+        <v>19.54</v>
       </c>
       <c r="J77" s="2">
-        <v>21.55</v>
+        <v>20.25</v>
       </c>
       <c r="K77" s="2">
-        <v>20.309999999999999</v>
+        <v>19.3</v>
       </c>
       <c r="L77" s="2">
-        <v>20.309999999999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>38</v>
@@ -3950,30 +3951,30 @@
         <v>10</v>
       </c>
       <c r="F78" s="2">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H78" s="2">
-        <v>20.46</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="I78" s="2">
-        <v>20.27</v>
+        <v>17.260000000000002</v>
       </c>
       <c r="J78" s="2">
-        <v>21.1</v>
+        <v>18.690000000000001</v>
       </c>
       <c r="K78" s="2">
-        <v>20.02</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="L78" s="2">
-        <v>20.399999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18.48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>38</v>
@@ -3988,30 +3989,30 @@
         <v>10</v>
       </c>
       <c r="F79" s="2">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H79" s="2">
-        <v>24.77</v>
+        <v>28.22</v>
       </c>
       <c r="I79" s="2">
-        <v>23.89</v>
+        <v>26.99</v>
       </c>
       <c r="J79" s="2">
-        <v>24.12</v>
+        <v>28.16</v>
       </c>
       <c r="K79" s="2">
-        <v>23.51</v>
+        <v>27.15</v>
       </c>
       <c r="L79" s="2">
-        <v>23.76</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26.41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>38</v>
@@ -4026,7 +4027,7 @@
         <v>10</v>
       </c>
       <c r="F80" s="2">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>85</v>
@@ -4035,21 +4036,21 @@
         <v>23.06</v>
       </c>
       <c r="I80" s="2">
-        <v>22.23</v>
+        <v>22.83</v>
       </c>
       <c r="J80" s="2">
-        <v>23.01</v>
+        <v>23.79</v>
       </c>
       <c r="K80" s="2">
-        <v>22.04</v>
+        <v>23.32</v>
       </c>
       <c r="L80" s="2">
-        <v>22.89</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>24.48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>38</v>
@@ -4058,34 +4059,34 @@
         <v>39</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F81" s="2">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H81" s="2">
-        <v>18.420000000000002</v>
+        <v>24.96</v>
       </c>
       <c r="I81" s="2">
-        <v>18.579999999999998</v>
+        <v>24.34</v>
       </c>
       <c r="J81" s="2">
-        <v>20.36</v>
+        <v>25.53</v>
       </c>
       <c r="K81" s="2">
-        <v>18.55</v>
+        <v>24.6</v>
       </c>
       <c r="L81" s="2">
-        <v>19.41</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25.53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>121</v>
       </c>
@@ -4108,7 +4109,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>122</v>
       </c>
@@ -4131,7 +4132,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>123</v>
       </c>
@@ -4154,7 +4155,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>124</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>125</v>
       </c>
@@ -4200,7 +4201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>126</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>127</v>
       </c>
@@ -4246,7 +4247,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -4269,7 +4270,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>129</v>
       </c>
@@ -4292,7 +4293,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>130</v>
       </c>
@@ -4315,7 +4316,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>131</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>132</v>
       </c>
@@ -4361,7 +4362,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>133</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>134</v>
       </c>
@@ -4407,7 +4408,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>135</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>136</v>
       </c>
@@ -4453,7 +4454,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>137</v>
       </c>
@@ -4476,7 +4477,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>138</v>
       </c>
@@ -4499,7 +4500,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -4522,7 +4523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>140</v>
       </c>
@@ -4545,7 +4546,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>141</v>
       </c>
@@ -4568,7 +4569,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>142</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>143</v>
       </c>
@@ -4614,7 +4615,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>144</v>
       </c>
@@ -4637,7 +4638,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>145</v>
       </c>
@@ -4660,7 +4661,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>146</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>147</v>
       </c>
@@ -4706,7 +4707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>148</v>
       </c>
@@ -4729,7 +4730,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>149</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>150</v>
       </c>
@@ -4775,7 +4776,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>151</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>152</v>
       </c>
@@ -4821,7 +4822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>153</v>
       </c>
@@ -4844,7 +4845,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>154</v>
       </c>
@@ -4867,7 +4868,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>155</v>
       </c>
@@ -4890,7 +4891,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>156</v>
       </c>
@@ -4913,7 +4914,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>157</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>158</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>159</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>160</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>161</v>
       </c>
@@ -5028,7 +5029,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>162</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>163</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>164</v>
       </c>
@@ -5097,7 +5098,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>165</v>
       </c>
@@ -5120,7 +5121,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>166</v>
       </c>
@@ -5143,7 +5144,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>167</v>
       </c>
@@ -5166,7 +5167,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>168</v>
       </c>
@@ -5189,7 +5190,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>169</v>
       </c>
@@ -5212,7 +5213,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>170</v>
       </c>
@@ -5235,7 +5236,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>171</v>
       </c>
@@ -5258,7 +5259,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>172</v>
       </c>
@@ -5281,7 +5282,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>173</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>174</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>175</v>
       </c>
@@ -5350,7 +5351,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>176</v>
       </c>
@@ -5373,7 +5374,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>177</v>
       </c>
@@ -5396,7 +5397,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>178</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>179</v>
       </c>
@@ -5442,7 +5443,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>180</v>
       </c>
@@ -5465,7 +5466,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>181</v>
       </c>
@@ -5488,7 +5489,7 @@
         <v>45859</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>182</v>
       </c>
@@ -5526,7 +5527,7 @@
         <v>19.61</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>185</v>
       </c>
@@ -5564,7 +5565,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>186</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>18.670000000000002</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>187</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>17.38</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>188</v>
       </c>
@@ -5678,7 +5679,7 @@
         <v>19.559999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>189</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>20.21</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>190</v>
       </c>
@@ -5754,7 +5755,7 @@
         <v>20.74</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>191</v>
       </c>
@@ -5792,7 +5793,7 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>192</v>
       </c>
@@ -5830,7 +5831,7 @@
         <v>21.01</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>193</v>
       </c>
@@ -5868,7 +5869,7 @@
         <v>19.27</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>194</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>195</v>
       </c>
@@ -5944,7 +5945,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>196</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>24.06</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>197</v>
       </c>
@@ -6020,7 +6021,7 @@
         <v>25.21</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>198</v>
       </c>
@@ -6058,7 +6059,7 @@
         <v>24.92</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>199</v>
       </c>
@@ -6096,7 +6097,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>200</v>
       </c>
@@ -6134,7 +6135,7 @@
         <v>23.86</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>201</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>202</v>
       </c>
@@ -6210,7 +6211,7 @@
         <v>23.56</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>203</v>
       </c>
@@ -6249,6 +6250,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L162" xr:uid="{2BF4FCBB-AC4B-4BE1-B463-C994B1598E3A}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="MYT1L"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:L81">
+      <sortCondition ref="A1:A162"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Myt1l L1 data added
</commit_message>
<xml_diff>
--- a/Data/Bandit paper Key.xlsx
+++ b/Data/Bandit paper Key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gowustl-my.sharepoint.com/personal/sebastiana_wustl_edu/Documents/Documents/GitHub/Murrell2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85C2E5E-8E87-42EE-B55E-7E56D2C4685E}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DBBA0D4-53C7-48F7-A7E5-291F6E3E412F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D69361D2-749D-4D5A-8D7C-5685B1F0A3DD}"/>
   </bookViews>
@@ -724,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -742,7 +742,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,6 +757,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1133,7 +1136,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>24.52</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>19.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>20.63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>27.35</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>20.23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>20.39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>23.59</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>26.05</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>19.809999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>23.87</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>25.54</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>20.420000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>20.079999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -3364,8 +3367,8 @@
         <v>19.41</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -3402,8 +3405,8 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>41</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -3440,8 +3443,8 @@
         <v>23.76</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>42</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -3478,8 +3481,8 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -3516,8 +3519,8 @@
         <v>20.309999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>44</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -3554,7 +3557,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>19.559999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -3630,7 +3633,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>21.11</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>26.04</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -3744,7 +3747,7 @@
         <v>26.94</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>50</v>
       </c>
@@ -3782,7 +3785,7 @@
         <v>20.45</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>51</v>
       </c>
@@ -3820,7 +3823,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>18.86</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -3896,7 +3899,7 @@
         <v>24.83</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>54</v>
       </c>
@@ -3934,7 +3937,7 @@
         <v>20.22</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -3972,7 +3975,7 @@
         <v>18.48</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>56</v>
       </c>
@@ -4010,7 +4013,7 @@
         <v>26.41</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -4048,7 +4051,7 @@
         <v>24.48</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>58</v>
       </c>
@@ -6253,7 +6256,7 @@
   <autoFilter ref="A1:L162" xr:uid="{2BF4FCBB-AC4B-4BE1-B463-C994B1598E3A}">
     <filterColumn colId="1">
       <filters>
-        <filter val="MYT1L"/>
+        <filter val="SHANK3B"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:L81">

</xml_diff>

<commit_message>
Nf1Cohort2 L1 organized Bandit 80
</commit_message>
<xml_diff>
--- a/Data/Bandit paper Key.xlsx
+++ b/Data/Bandit paper Key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gowustl-my.sharepoint.com/personal/sebastiana_wustl_edu/Documents/Documents/GitHub/Murrell2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="218" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61EC67B2-6B6B-48BF-9A54-391CF1BFB348}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{F8E0B11F-43C0-4782-8D95-C5B9BD28F34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24D3E4B9-315D-41E9-AEEC-99D40A62FEC6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D69361D2-749D-4D5A-8D7C-5685B1F0A3DD}"/>
   </bookViews>
@@ -754,6 +754,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1829,7 +1833,7 @@
         <v>19.68</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>24.28</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1905,7 +1909,7 @@
         <v>19.64</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>19.98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>18.350000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2051,7 +2055,7 @@
         <v>25.66</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>19.38</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>17.850000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2156,7 +2160,7 @@
         <v>21.05</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2191,7 +2195,7 @@
         <v>23.02</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2226,7 +2230,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2261,7 +2265,7 @@
         <v>22.38</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>19.62</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2337,7 +2341,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2375,7 +2379,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -2413,7 +2417,7 @@
         <v>25.25</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>17.86</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2486,7 +2490,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2524,7 +2528,7 @@
         <v>27.32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>101</v>
       </c>
@@ -2562,7 +2566,7 @@
         <v>18.559999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2600,7 +2604,7 @@
         <v>20.71</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>18.97</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2676,7 +2680,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2714,7 +2718,7 @@
         <v>21.47</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>21.21</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -2790,7 +2794,7 @@
         <v>26.39</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -2828,7 +2832,7 @@
         <v>25.88</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>116</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>24.56</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>118</v>
       </c>
@@ -2904,7 +2908,7 @@
         <v>24.38</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>114</v>
       </c>
@@ -2942,7 +2946,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2980,7 +2984,7 @@
         <v>27.91</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3018,7 +3022,7 @@
         <v>19.079999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -3056,7 +3060,7 @@
         <v>19.77</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -3094,7 +3098,7 @@
         <v>26.07</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -3132,7 +3136,7 @@
         <v>18.88</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -3208,7 +3212,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -6211,10 +6215,10 @@
   <autoFilter ref="A1:L161" xr:uid="{2BF4FCBB-AC4B-4BE1-B463-C994B1598E3A}">
     <filterColumn colId="1">
       <filters>
-        <filter val="DNMT3a"/>
+        <filter val="NF1Cohort 2"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A142:L161">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:L60">
       <sortCondition ref="A1:A161"/>
     </sortState>
   </autoFilter>

</xml_diff>